<commit_message>
Store datasets with Git LFS
</commit_message>
<xml_diff>
--- a/model/denetimli/result.xlsx
+++ b/model/denetimli/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
   <si>
     <t>Sonuçlar</t>
   </si>
@@ -94,9 +94,6 @@
     <t>MLP</t>
   </si>
   <si>
-    <t>SVM</t>
-  </si>
-  <si>
     <t>TCN</t>
   </si>
   <si>
@@ -110,6 +107,222 @@
   </si>
   <si>
     <t>LSTM Autoencoder</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.9972</t>
+  </si>
+  <si>
+    <t>0.9427</t>
+  </si>
+  <si>
+    <t>0.9083</t>
+  </si>
+  <si>
+    <t>0.9252</t>
+  </si>
+  <si>
+    <t>0.0028</t>
+  </si>
+  <si>
+    <t>0.9986</t>
+  </si>
+  <si>
+    <t>0.9799</t>
+  </si>
+  <si>
+    <t>0.9437</t>
+  </si>
+  <si>
+    <t>0.9615</t>
+  </si>
+  <si>
+    <t>0.0014</t>
+  </si>
+  <si>
+    <t>Streaming Logistic-SGD</t>
+  </si>
+  <si>
+    <t>0.9391</t>
+  </si>
+  <si>
+    <t>0.9890</t>
+  </si>
+  <si>
+    <t>0.7745</t>
+  </si>
+  <si>
+    <t>0.6010</t>
+  </si>
+  <si>
+    <t>0.6768</t>
+  </si>
+  <si>
+    <t>0.0110</t>
+  </si>
+  <si>
+    <t>0.990</t>
+  </si>
+  <si>
+    <t>0.8887</t>
+  </si>
+  <si>
+    <t>0.0579</t>
+  </si>
+  <si>
+    <t>0.3165</t>
+  </si>
+  <si>
+    <t>0.0979</t>
+  </si>
+  <si>
+    <t>0.1113</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.9981</t>
+  </si>
+  <si>
+    <t>0.9674</t>
+  </si>
+  <si>
+    <t>0.9293</t>
+  </si>
+  <si>
+    <t>0.9480</t>
+  </si>
+  <si>
+    <t>0.0019</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>ExtraTrees</t>
+  </si>
+  <si>
+    <t>HistGradientBoostingClassifier</t>
+  </si>
+  <si>
+    <t>GradientBoostingClassifier</t>
+  </si>
+  <si>
+    <t>AdaBoostClassifier</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>DecisionTreeClassifier</t>
+  </si>
+  <si>
+    <t>Gaussian Naive Bayes</t>
+  </si>
+  <si>
+    <t>0.9994</t>
+  </si>
+  <si>
+    <t>0.9997</t>
+  </si>
+  <si>
+    <t>0.9998</t>
+  </si>
+  <si>
+    <t>0.9917</t>
+  </si>
+  <si>
+    <t>0.9958</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>0.9995</t>
+  </si>
+  <si>
+    <t>0.9996</t>
+  </si>
+  <si>
+    <t>0.9991</t>
+  </si>
+  <si>
+    <t>0.9602</t>
+  </si>
+  <si>
+    <t>0.9962</t>
+  </si>
+  <si>
+    <t>0.9779</t>
+  </si>
+  <si>
+    <t>0.0009</t>
+  </si>
+  <si>
+    <t>0.9574</t>
+  </si>
+  <si>
+    <t>0.3093</t>
+  </si>
+  <si>
+    <t>0.4725</t>
+  </si>
+  <si>
+    <t>0.0426</t>
+  </si>
+  <si>
+    <t>0.003685</t>
+  </si>
+  <si>
+    <t>0.9713</t>
+  </si>
+  <si>
+    <t>0.3390</t>
+  </si>
+  <si>
+    <t>0.5290</t>
+  </si>
+  <si>
+    <t>0.4132</t>
+  </si>
+  <si>
+    <t>0.0287</t>
+  </si>
+  <si>
+    <t>model sonuçları</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>QSVM</t>
+  </si>
+  <si>
+    <t>VQC</t>
+  </si>
+  <si>
+    <t>PegasosQSVC</t>
+  </si>
+  <si>
+    <t>QSVR</t>
+  </si>
+  <si>
+    <t>VQR</t>
+  </si>
+  <si>
+    <t>NeuralNetworkClassifier</t>
+  </si>
+  <si>
+    <t>QCNN</t>
+  </si>
+  <si>
+    <t>QuantumAutoencoder</t>
   </si>
 </sst>
 </file>
@@ -502,12 +715,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -516,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -552,7 +823,9 @@
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>4759</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -564,7 +837,9 @@
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>405748</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -576,7 +851,9 @@
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>1386</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -588,7 +865,9 @@
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <v>3159</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -600,7 +879,9 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -612,7 +893,9 @@
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -624,7 +907,9 @@
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -636,7 +921,9 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -648,7 +935,9 @@
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -660,7 +949,9 @@
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -670,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>0</v>
@@ -686,7 +977,9 @@
       <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4">
+        <v>7358</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -698,7 +991,9 @@
       <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>406767</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -710,7 +1005,9 @@
       <c r="D16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>248</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -722,7 +1019,9 @@
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>560</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -734,7 +1033,9 @@
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -746,7 +1047,9 @@
       <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -758,7 +1061,9 @@
       <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -770,7 +1075,9 @@
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -782,7 +1089,9 @@
       <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
@@ -794,7 +1103,9 @@
       <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
@@ -802,13 +1113,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>0</v>
@@ -818,101 +1129,141 @@
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4">
+        <v>7192</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4">
+        <v>7472</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4">
+        <v>406578</v>
+      </c>
       <c r="D27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4">
+        <v>406862</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4">
+        <v>437</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>153</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4">
+        <v>726</v>
+      </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>446</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="D34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
@@ -922,13 +1273,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>0</v>
@@ -938,101 +1289,141 @@
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4">
+        <v>2506</v>
+      </c>
       <c r="D38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4">
+        <v>4189</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="4"/>
+      <c r="B39" s="4">
+        <v>366255</v>
+      </c>
       <c r="D39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4">
+        <v>398846</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>40760</v>
+      </c>
       <c r="D40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4">
+        <v>8169</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="4">
+        <v>5412</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>3729</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="D43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1042,28 +1433,1114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7913</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>407134</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>407134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>7916</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>7918</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4">
+        <v>407130</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>407134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4">
+        <v>7918</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4">
+        <v>7888</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4">
+        <v>407134</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>406807</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4">
+        <v>7918</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4">
+        <v>7918</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4">
+        <v>407134</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>389454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="4">
+        <v>17680</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="D28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="D32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="D36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="D41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="D43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="D45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="D46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="D49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>